<commit_message>
code till search particular application
</commit_message>
<xml_diff>
--- a/Angel_Broking/Angel/DriverFile/ApplicationData.xlsx
+++ b/Angel_Broking/Angel/DriverFile/ApplicationData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Offline_Journey_Tab</t>
+  </si>
+  <si>
+    <t>Scrutiny_Page</t>
   </si>
   <si>
     <t>TC001</t>
@@ -78,9 +81,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -106,14 +109,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,30 +117,38 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,26 +162,56 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,9 +225,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,45 +238,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +260,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -275,79 +272,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,91 +440,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,6 +484,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -505,8 +511,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,15 +528,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,154 +561,154 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -724,7 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -734,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1058,7 +1055,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1071,7 +1068,7 @@
     <col min="6" max="6" width="17.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:10">
+    <row r="1" s="1" customFormat="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1102,39 +1099,44 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5"/>

</xml_diff>